<commit_message>
Fix hotbox power issue and cable miscount
</commit_message>
<xml_diff>
--- a/events/anw/2023/ANW2023.xlsx
+++ b/events/anw/2023/ANW2023.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PowerCables" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t xml:space="preserve">Power</t>
   </si>
@@ -537,8 +537,8 @@
   </sheetPr>
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -781,11 +781,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="n">
-        <v>0.13</v>
+        <v>0.68</v>
       </c>
       <c r="D7" s="10" t="n">
         <f aca="false">C7*B7</f>
-        <v>0.26</v>
+        <v>1.36</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -856,14 +856,14 @@
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="n">
         <f aca="false">SUM(D5:D8)</f>
-        <v>4.05</v>
+        <v>5.15</v>
       </c>
       <c r="E9" s="15" t="n">
         <f aca="false">D9*8</f>
-        <v>32.4</v>
+        <v>41.2</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
@@ -967,11 +967,11 @@
         <v>2</v>
       </c>
       <c r="C12" s="10" t="n">
-        <v>0.13</v>
+        <v>0.68</v>
       </c>
       <c r="D12" s="10" t="n">
         <f aca="false">C12*B12</f>
-        <v>0.26</v>
+        <v>1.36</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1012,8 +1012,8 @@
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="11" t="s">
-        <v>8</v>
+      <c r="G13" s="11" t="n">
+        <v>4</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -1039,11 +1039,11 @@
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="n">
         <f aca="false">SUM(D11:D13)</f>
-        <v>1.75</v>
+        <v>2.85</v>
       </c>
       <c r="E14" s="15" t="n">
         <f aca="false">D14*4</f>
-        <v>7</v>
+        <v>11.4</v>
       </c>
       <c r="F14" s="15" t="n">
         <v>1</v>
@@ -1833,7 +1833,7 @@
       <c r="D39" s="10"/>
       <c r="E39" s="10" t="n">
         <f aca="false">SUM(E4:E38)</f>
-        <v>94.388</v>
+        <v>107.588</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="11"/>
@@ -1863,11 +1863,11 @@
       </c>
       <c r="F40" s="10" t="n">
         <f aca="false">SUM(F3:F39)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G40" s="11" t="n">
         <f aca="false">SUM(G3:G38)</f>
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H40" s="11" t="n">
         <f aca="false">SUM(H3:H38)</f>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="G44" s="9" t="n">
         <f aca="false">ROUND(G40*1.05,0)</f>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="H44" s="9" t="n">
         <f aca="false">ROUND(H40*1.05,0)</f>
@@ -2131,8 +2131,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>